<commit_message>
export xsl and csv for propertyfiles added in admin actions
</commit_message>
<xml_diff>
--- a/version plan.xlsx
+++ b/version plan.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\feetracker\feetracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5DE400-2E61-4E90-B33A-93A2FF3414CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="version discription" sheetId="2" r:id="rId1"/>
     <sheet name="task list" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'task list'!$A$1:$D$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'task list'!$A$1:$D$16</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>category</t>
   </si>
@@ -214,23 +215,26 @@
   </si>
   <si>
     <t>3.5.4</t>
+  </si>
+  <si>
+    <t>chenge the logic to build one fundamental grid search once a day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -238,7 +242,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -386,10 +390,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,11 +424,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="version"/>
-    <tableColumn id="2" name="comment"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="version"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -692,20 +696,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7890625" customWidth="1"/>
-    <col min="2" max="2" width="32.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.75" customWidth="1"/>
+    <col min="2" max="2" width="32.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -713,7 +717,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -721,7 +725,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -729,7 +733,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -737,7 +741,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -751,23 +755,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.3" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="109.734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.20703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83984375" style="22"/>
+    <col min="1" max="1" width="109.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -784,7 +788,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -797,13 +801,13 @@
       <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -814,28 +818,26 @@
       <c r="D3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="D4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
@@ -846,45 +848,45 @@
       <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="E5" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A7" s="3" t="s">
-        <v>43</v>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="22"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="D7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>40</v>
@@ -895,28 +897,28 @@
       <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A9" s="11" t="s">
+      <c r="E8" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5">
-        <v>3</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A10" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -927,28 +929,28 @@
       <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="E10" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="5">
-        <v>3</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A12" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>4</v>
@@ -956,33 +958,33 @@
       <c r="C12" s="5">
         <v>3</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A13" s="7" t="s">
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="5">
-        <v>3</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A14" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>6</v>
@@ -993,11 +995,13 @@
       <c r="D14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="E14" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>6</v>
@@ -1006,32 +1010,30 @@
         <v>3</v>
       </c>
       <c r="D15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E16" s="20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="5">
-        <v>3</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A17" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>38</v>
@@ -1042,65 +1044,65 @@
       <c r="D17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="21"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="E17" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5">
+        <v>3</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="22"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="5">
-        <v>3</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="20" t="s">
+      <c r="B19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>3</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A19" s="7" t="s">
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="5">
-        <v>3</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="B20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="5">
+        <v>3</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E20" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" s="5">
-        <v>3</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="C21" s="5">
         <v>3</v>
@@ -1109,12 +1111,12 @@
         <v>10</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>5</v>
@@ -1126,41 +1128,58 @@
         <v>10</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="5">
-        <v>3</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="20" t="s">
+      <c r="C24" s="5">
+        <v>3</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="20" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D15"/>
-  <sortState ref="A2:E23">
+  <autoFilter ref="A1:D16" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <sortState ref="A2:E24">
     <sortCondition ref="C1"/>
   </sortState>
   <mergeCells count="6">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>